<commit_message>
Executable is present in Final.exe Modified others
</commit_message>
<xml_diff>
--- a/Data_analysis/UT_data/program_Ford_DCME_metric.xlsx
+++ b/Data_analysis/UT_data/program_Ford_DCME_metric.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Files\git_Python\Data_analysis\UT_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT FILES\git_Python\Data_analysis\UT_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E5ED35-3E45-4AD4-883B-5535309C854B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B43C36F-1553-4110-9BD9-DC1CD82171D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HIS (Routines)" sheetId="1" r:id="rId1"/>
+    <sheet name="HIS (Classes,Methods,Types)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="52">
   <si>
     <t>Entity</t>
   </si>
@@ -500,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,4 +935,440 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B28184D-09BE-4FEC-8053-CC81B13728B3}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>